<commit_message>
Demo2 Version2 (Self generate model soruce)
</commit_message>
<xml_diff>
--- a/CenterCLR.Demo2/csvdefinition.xlsx
+++ b/CenterCLR.Demo2/csvdefinition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>カラム名</t>
     <rPh sb="3" eb="4">
@@ -51,20 +51,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>苗字</t>
-    <rPh sb="0" eb="2">
-      <t>ミョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>名前</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>郵便番号</t>
     <rPh sb="0" eb="4">
       <t>ユウビンバンゴウ</t>
@@ -72,102 +58,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>都道府県</t>
-    <rPh sb="0" eb="4">
-      <t>トドウフケン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>市区町村</t>
-    <rPh sb="0" eb="2">
-      <t>シク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>チョウソン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>住所１</t>
-    <rPh sb="0" eb="2">
-      <t>ジュウショ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>住所２</t>
-    <rPh sb="0" eb="2">
-      <t>ジュウショ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>電話番号</t>
-    <rPh sb="0" eb="2">
-      <t>デンワ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>バンゴウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>生年月日</t>
-    <rPh sb="0" eb="2">
-      <t>セイネン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ガッピ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>登録日</t>
-    <rPh sb="0" eb="3">
-      <t>トウロクビ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>パスワード</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>SALT</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メモ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サインインID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>苗字のみ</t>
-    <rPh sb="0" eb="2">
-      <t>ミョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>名前のみ</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>123-4567</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>文字列</t>
     <rPh sb="0" eb="3">
       <t>モジレツ</t>
@@ -175,42 +65,267 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>文字列（ハイフンあり）</t>
-    <rPh sb="0" eb="3">
-      <t>モジレツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>西暦</t>
-    <rPh sb="0" eb="2">
-      <t>セイレキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HMAC-SHA1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>KEY</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>64ビット整数</t>
+    <t>コード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全国地方公共団体コード</t>
+    <rPh sb="0" eb="2">
+      <t>ゼンコク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>チホウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>コウキョウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ダンタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>32ビット整数</t>
     <rPh sb="5" eb="7">
       <t>セイスウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>DateTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バイト列</t>
-    <rPh sb="3" eb="4">
-      <t>レツ</t>
+    <t>旧郵便番号</t>
+    <rPh sb="0" eb="1">
+      <t>キュウ</t>
+    </rPh>
+    <rPh sb="1" eb="5">
+      <t>ユウビンバンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5桁</t>
+    <rPh sb="1" eb="2">
+      <t>ケタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7桁</t>
+    <rPh sb="1" eb="2">
+      <t>ケタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>都道府県名</t>
+    <rPh sb="0" eb="4">
+      <t>トドウフケン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>半角カナ</t>
+    <rPh sb="0" eb="2">
+      <t>ハンカク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市区町村名</t>
+    <rPh sb="0" eb="2">
+      <t>シク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>チョウソン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>町域名</t>
+    <rPh sb="0" eb="2">
+      <t>チョウイキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>漢字</t>
+    <rPh sb="0" eb="2">
+      <t>カンジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>都道府県カナ名</t>
+    <rPh sb="0" eb="4">
+      <t>トドウフケン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市区町村カナ名</t>
+    <rPh sb="0" eb="2">
+      <t>シク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>チョウソン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>町域カナ名</t>
+    <rPh sb="0" eb="2">
+      <t>チョウイキ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>重郵便番号</t>
+    <rPh sb="0" eb="1">
+      <t>ジュウ</t>
+    </rPh>
+    <rPh sb="1" eb="5">
+      <t>ユウビンバンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>小字別町域</t>
+    <rPh sb="0" eb="2">
+      <t>コアザ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>チョウイキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フラグ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>真偽値</t>
+    <rPh sb="0" eb="2">
+      <t>シンギ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>丁目</t>
+    <rPh sb="0" eb="2">
+      <t>チョウメ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>重町域</t>
+    <rPh sb="0" eb="1">
+      <t>ジュウ</t>
+    </rPh>
+    <rPh sb="1" eb="3">
+      <t>チョウイキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:変更なし, 1:変更あり, 2:廃止</t>
+    <rPh sb="2" eb="4">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ハイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8ビット整数</t>
+    <rPh sb="4" eb="6">
+      <t>セイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更理由</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>リユウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:変更なし, 1:指令都市施行, 2:住居表示, 3:区画整理, 4:郵便区調整, 5:訂正, 6:廃止</t>
+    <rPh sb="2" eb="4">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シレイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>トシ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シコウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ジュウキョ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>クカク</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セイリ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ユウビン</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>チョウセイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>テイセイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ハイシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -283,8 +398,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル1" displayName="テーブル1" ref="A1:D16" totalsRowShown="0">
+  <autoFilter ref="A1:D16"/>
   <tableColumns count="4">
     <tableColumn id="1" name="No"/>
     <tableColumn id="2" name="カラム名"/>
@@ -558,7 +673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -567,7 +682,7 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="39.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
@@ -591,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,13 +720,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,13 +734,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,13 +748,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,13 +762,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,13 +776,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,13 +790,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,13 +804,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -703,13 +818,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -717,13 +832,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -731,13 +846,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -745,13 +860,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -759,13 +874,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
         <v>25</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -773,13 +888,27 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo2 Version 3 (Predefined column index metadata by custom attributes)
</commit_message>
<xml_diff>
--- a/CenterCLR.Demo2/csvdefinition.xlsx
+++ b/CenterCLR.Demo2/csvdefinition.xlsx
@@ -676,7 +676,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -703,7 +703,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>

</xml_diff>